<commit_message>
Codigo Mejorado POT digtal
</commit_message>
<xml_diff>
--- a/Estimulador/Caracterizacion/Tablas_Resultados.xlsx
+++ b/Estimulador/Caracterizacion/Tablas_Resultados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Universidad UVG\Sexto Año\Segundo Ciclo\Tesis\Tesis-2022-Erick-Aquino\Estimulador\Caracterizacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E59C268-2DAE-46F8-9B25-3097BF162039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9C75A3-8F7A-4429-959A-3838B2B101B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{EFFD592A-B6F9-484D-AA51-F79BFFF83EBA}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>Error (%)</t>
   </si>
@@ -81,6 +81,51 @@
   <si>
     <t>Amplitud experimental (V)</t>
   </si>
+  <si>
+    <t>Amplitud</t>
+  </si>
+  <si>
+    <t>Amplitud experimental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frecuencia (Hz) </t>
+  </si>
+  <si>
+    <t>Exp Frecuencia (Hz)</t>
+  </si>
+  <si>
+    <t>Error Frecuencia (%)</t>
+  </si>
+  <si>
+    <t>Error Amplitud (%)</t>
+  </si>
+  <si>
+    <t>error tiempo de subida (%)</t>
+  </si>
+  <si>
+    <t>Promedio Bajada (ms)</t>
+  </si>
+  <si>
+    <t>error bajada (%)</t>
+  </si>
+  <si>
+    <t>DUTY CYCLE 50%</t>
+  </si>
+  <si>
+    <t>DUTY CYCLE 55%</t>
+  </si>
+  <si>
+    <t>DUTY CYCLE 20%</t>
+  </si>
+  <si>
+    <t>Tiempo Rampa Subida Teorico (s)</t>
+  </si>
+  <si>
+    <t>Tiempo Rampa Bajada (s)</t>
+  </si>
+  <si>
+    <t>Promedio subida (s)</t>
+  </si>
 </sst>
 </file>
 
@@ -89,7 +134,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,8 +149,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +166,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -132,7 +189,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -158,20 +215,167 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+  <dxfs count="61">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -179,13 +383,13 @@
       <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -428,48 +632,141 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4DB0725B-06C7-40AB-8951-220298407BB2}" name="Tabla1" displayName="Tabla1" ref="A1:J23" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4DB0725B-06C7-40AB-8951-220298407BB2}" name="Tabla1" displayName="Tabla1" ref="A1:J23" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="A1:J23" xr:uid="{4DB0725B-06C7-40AB-8951-220298407BB2}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{D8BE834C-C6A0-4D47-BBA1-05DAD44C12B6}" name="Frequencia PWM Teorica (Hz)" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{E3D22371-E809-4283-A1E6-06CCF407C76F}" name="Pomedio PWM (Hz)" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{27EE4F05-B556-4BCF-B7F8-6EDA21BE7791}" name="Error (%)" dataDxfId="14" dataCellStyle="Porcentaje">
+    <tableColumn id="1" xr3:uid="{D8BE834C-C6A0-4D47-BBA1-05DAD44C12B6}" name="Frequencia PWM Teorica (Hz)" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{E3D22371-E809-4283-A1E6-06CCF407C76F}" name="Pomedio PWM (Hz)" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{27EE4F05-B556-4BCF-B7F8-6EDA21BE7791}" name="Error (%)" dataDxfId="56" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>ABS((Tabla1[[#This Row],[Pomedio PWM (Hz)]]-Tabla1[[#This Row],[Frequencia PWM Teorica (Hz)]])/Tabla1[[#This Row],[Frequencia PWM Teorica (Hz)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C87F5F2D-3C48-4667-A3F8-31665B839217}" name="Ciclo de trabajo teorico" dataDxfId="13" dataCellStyle="Porcentaje"/>
-    <tableColumn id="9" xr3:uid="{D2FC5D2D-9F0F-40CD-92B9-A87E4EF0119F}" name="Promedio ciclo de trabajo (%)" dataDxfId="12" dataCellStyle="Porcentaje"/>
-    <tableColumn id="10" xr3:uid="{5ED67E0A-997F-46E6-BF33-45D8CF858762}" name="Error ciclo de trabajo (%)" dataDxfId="11" dataCellStyle="Porcentaje">
+    <tableColumn id="8" xr3:uid="{C87F5F2D-3C48-4667-A3F8-31665B839217}" name="Ciclo de trabajo teorico" dataDxfId="55" dataCellStyle="Porcentaje"/>
+    <tableColumn id="9" xr3:uid="{D2FC5D2D-9F0F-40CD-92B9-A87E4EF0119F}" name="Promedio ciclo de trabajo (%)" dataDxfId="54" dataCellStyle="Porcentaje"/>
+    <tableColumn id="10" xr3:uid="{5ED67E0A-997F-46E6-BF33-45D8CF858762}" name="Error ciclo de trabajo (%)" dataDxfId="53" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>ABS((Tabla1[[#This Row],[Promedio ciclo de trabajo (%)]]-Tabla1[[#This Row],[Ciclo de trabajo teorico]])/Tabla1[[#This Row],[Ciclo de trabajo teorico]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E6A42BD8-6B1E-494C-92D0-8809E4C6E417}" name="Ancho de pulso teorico (ms)" dataDxfId="10">
+    <tableColumn id="4" xr3:uid="{E6A42BD8-6B1E-494C-92D0-8809E4C6E417}" name="Ancho de pulso teorico (ms)" dataDxfId="52">
       <calculatedColumnFormula>(1/Tabla1[[#This Row],[Frequencia PWM Teorica (Hz)]])*Tabla1[[#This Row],[Ciclo de trabajo teorico]]*1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{18FA8CF7-1748-4290-934F-195BB10A3E9D}" name="Promedio Ancho de pulso (ms)" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{8C38799C-6282-4F30-8155-2F925A8104B1}" name="Error ancho de pulso (%)" dataDxfId="8" dataCellStyle="Porcentaje">
+    <tableColumn id="6" xr3:uid="{18FA8CF7-1748-4290-934F-195BB10A3E9D}" name="Promedio Ancho de pulso (ms)" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{8C38799C-6282-4F30-8155-2F925A8104B1}" name="Error ancho de pulso (%)" dataDxfId="50" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>ABS((Tabla1[[#This Row],[Promedio Ancho de pulso (ms)]]-Tabla1[[#This Row],[Ancho de pulso teorico (ms)]])/Tabla1[[#This Row],[Ancho de pulso teorico (ms)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1B8DFAA5-0DC3-4A17-85A3-B56B9D035E8D}" name="voltaje (v)" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{1B8DFAA5-0DC3-4A17-85A3-B56B9D035E8D}" name="voltaje (v)" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{541620B9-3328-4E80-87D7-6993CCFCC757}" name="Tabla2" displayName="Tabla2" ref="A1:E16" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{541620B9-3328-4E80-87D7-6993CCFCC757}" name="Tabla2" displayName="Tabla2" ref="A1:E16" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <autoFilter ref="A1:E16" xr:uid="{541620B9-3328-4E80-87D7-6993CCFCC757}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C17AFB38-CE22-46D7-8F22-0682A82000DC}" name="Amplitud  teórica (V)" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{C17AFB38-CE22-46D7-8F22-0682A82000DC}" name="Amplitud  teórica (V)" dataDxfId="46">
       <calculatedColumnFormula>A1-0.25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{CAC73A74-053C-4BEA-BFA3-0EF61C871549}" name="Amplitud experimental (V)" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{58572678-C524-4439-815F-B36F210BCB44}" name="Error (%)" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{CAC73A74-053C-4BEA-BFA3-0EF61C871549}" name="Amplitud experimental (V)" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{58572678-C524-4439-815F-B36F210BCB44}" name="Error (%)" dataDxfId="44">
       <calculatedColumnFormula>ABS((Tabla2[[#This Row],[Amplitud experimental (V)]]-Tabla2[[#This Row],[Amplitud  teórica (V)]])/Tabla2[[#This Row],[Amplitud  teórica (V)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C3BEE760-7C9E-4D95-A987-D6B7F4281D8C}" name="Potenciometro (%)" dataDxfId="0" dataCellStyle="Porcentaje">
+    <tableColumn id="4" xr3:uid="{C3BEE760-7C9E-4D95-A987-D6B7F4281D8C}" name="Potenciometro (%)" dataDxfId="43" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>(Tabla2[[#This Row],[Value sent (0 - 255)]]*100/255)*0.01</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{6E5851DF-90B5-4596-B293-DB5BB1C46723}" name="Value sent (0 - 255)" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{6E5851DF-90B5-4596-B293-DB5BB1C46723}" name="Value sent (0 - 255)" dataDxfId="42">
       <calculatedColumnFormula>Tabla2[[#This Row],[Amplitud  teórica (V)]]*255/3.3</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5BBDF8BE-AC6E-4031-9579-29D05467F7BF}" name="Tabla3" displayName="Tabla3" ref="A2:L17" totalsRowShown="0" headerRowDxfId="41" dataDxfId="34">
+  <autoFilter ref="A2:L17" xr:uid="{5BBDF8BE-AC6E-4031-9579-29D05467F7BF}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{9F71D84F-9878-4D36-8936-9D003F31027F}" name="Frecuencia (Hz) " dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{5282C3EA-F82F-4E75-BDCF-1084006587B3}" name="Exp Frecuencia (Hz)" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{ED172ABE-988C-4750-854D-F9F0691C9376}" name="Error Frecuencia (%)" dataDxfId="32" dataCellStyle="Porcentaje">
+      <calculatedColumnFormula>ABS((Tabla3[[#This Row],[Exp Frecuencia (Hz)]]-Tabla3[[#This Row],[Frecuencia (Hz) ]])/Tabla3[[#This Row],[Frecuencia (Hz) ]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{88E66329-9A9A-4F1D-81CC-884B1C7872B9}" name="Amplitud" dataDxfId="38"/>
+    <tableColumn id="11" xr3:uid="{09F1E6EF-B67B-451B-9DE2-1EE82D3585CB}" name="Amplitud experimental" dataDxfId="33"/>
+    <tableColumn id="12" xr3:uid="{C80D96D2-FC0F-48F2-9D46-C0DFF83B2CD7}" name="Error Amplitud (%)" dataDxfId="31">
+      <calculatedColumnFormula>ABS((Tabla3[[#This Row],[Amplitud experimental]]-Tabla3[[#This Row],[Amplitud]])/Tabla3[[#This Row],[Amplitud]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{D4F0D9EB-B70D-4932-A0EB-05BFE46B43ED}" name="Tiempo Rampa Subida Teorico (s)" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{2EBD1AB8-5FE1-4887-AE3B-19D56A70A9EF}" name="Promedio subida (s)" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{CCAC1463-901C-4C7D-A762-180D99650D11}" name="error tiempo de subida (%)" dataDxfId="30">
+      <calculatedColumnFormula>ABS((Tabla3[[#This Row],[Promedio subida (s)]]-Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{30C74FAF-B5D2-44CA-BF59-EB5E6D7B1A9C}" name="Tiempo Rampa Bajada (s)" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{1891CEE3-E6E8-47C1-98E4-60A57F883566}" name="Promedio Bajada (ms)" dataDxfId="28">
+      <calculatedColumnFormula>Tabla3[[#This Row],[Promedio subida (s)]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{16438C67-DAE6-4F33-8725-B2B824DE7049}" name="error bajada (%)" dataDxfId="29">
+      <calculatedColumnFormula>ABS((Tabla3[[#This Row],[Promedio Bajada (ms)]]-Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{04551ECA-EF0C-4696-9301-5248DE3C38A9}" name="Tabla311" displayName="Tabla311" ref="A22:L37" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A22:L37" xr:uid="{04551ECA-EF0C-4696-9301-5248DE3C38A9}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{954A970E-0EE2-41A4-96CD-DF54CD9B89BD}" name="Frecuencia (Hz) " dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{4F819BC9-EAF4-4102-98E5-2D695C220C79}" name="Exp Frecuencia (Hz)" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{3EA23BCF-637E-4183-951D-AE5A4E1B4996}" name="Error Frecuencia (%)" dataDxfId="23" dataCellStyle="Porcentaje">
+      <calculatedColumnFormula>ABS((Tabla311[[#This Row],[Exp Frecuencia (Hz)]]-Tabla311[[#This Row],[Frecuencia (Hz) ]])/Tabla311[[#This Row],[Frecuencia (Hz) ]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{57FDEE6C-38A0-4878-90E5-D462DC893965}" name="Amplitud" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{A1EA1D9B-8E35-45C2-BC97-1F7531639C8E}" name="Amplitud experimental" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{5C5B86F0-2C62-4EC7-90DB-16CD3F02F215}" name="Error Amplitud (%)" dataDxfId="20">
+      <calculatedColumnFormula>ABS((Tabla311[[#This Row],[Amplitud experimental]]-Tabla311[[#This Row],[Amplitud]])/Tabla311[[#This Row],[Amplitud]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{A196DC78-24A3-49DB-8F89-7372B726AF8D}" name="Tiempo Rampa Subida Teorico (s)" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{61205670-DD09-4734-9B60-2A19181A3B09}" name="Promedio subida (s)" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{CB6D4961-C564-4255-A528-66DC8939E53F}" name="error tiempo de subida (%)" dataDxfId="17">
+      <calculatedColumnFormula>ABS((Tabla311[[#This Row],[Promedio subida (s)]]-Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{82C89E9A-C54F-45D9-BA16-F7CA53FDAD9C}" name="Tiempo Rampa Bajada (s)" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{AADECCD1-0E47-4899-B4DB-3980D5EB4FA0}" name="Promedio Bajada (ms)" dataDxfId="15">
+      <calculatedColumnFormula>Tabla311[[#This Row],[Promedio subida (s)]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{B9442908-7763-415B-A1D9-3FDB69AA335D}" name="error bajada (%)" dataDxfId="14">
+      <calculatedColumnFormula>ABS((Tabla311[[#This Row],[Promedio Bajada (ms)]]-Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{FD84326B-B51B-43E3-A954-A199DB93B556}" name="Tabla312" displayName="Tabla312" ref="A41:L56" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A41:L56" xr:uid="{FD84326B-B51B-43E3-A954-A199DB93B556}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{9EA3655E-189F-41AE-BB30-A54F6B6FBD31}" name="Frecuencia (Hz) " dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{43A90E76-0F57-46ED-9A57-AA589374EFAC}" name="Exp Frecuencia (Hz)" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{402459F6-1584-430A-83A0-BCD4F9F04646}" name="Error Frecuencia (%)" dataDxfId="9" dataCellStyle="Porcentaje">
+      <calculatedColumnFormula>ABS((Tabla312[[#This Row],[Exp Frecuencia (Hz)]]-Tabla312[[#This Row],[Frecuencia (Hz) ]])/Tabla312[[#This Row],[Frecuencia (Hz) ]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{57E12FE0-ED8A-4975-B183-AD60486386D0}" name="Amplitud" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{8BB747FA-A49A-40D7-8EB0-CE09BDEFD4C6}" name="Amplitud experimental" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{5AD41EFA-DE50-4D69-927C-30DDC6471368}" name="Error Amplitud (%)" dataDxfId="6">
+      <calculatedColumnFormula>ABS((Tabla312[[#This Row],[Amplitud experimental]]-Tabla312[[#This Row],[Amplitud]])/Tabla312[[#This Row],[Amplitud]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{8F77CD90-8B24-4F57-B9D9-D92BD38EEF90}" name="Tiempo Rampa Subida Teorico (s)" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{369A3313-8A54-4DE9-ABDF-57550D7CA766}" name="Promedio subida (s)" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{623ED2C3-F247-4060-B588-027666E64CEF}" name="error tiempo de subida (%)" dataDxfId="3">
+      <calculatedColumnFormula>ABS((Tabla312[[#This Row],[Promedio subida (s)]]-Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{E3C34122-9074-4143-952B-814317832A8D}" name="Tiempo Rampa Bajada (s)" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{60537B1A-AA51-4135-9C45-7A7737C1206F}" name="Promedio Bajada (ms)" dataDxfId="1">
+      <calculatedColumnFormula>Tabla312[[#This Row],[Promedio subida (s)]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{AC06E1BE-4CD9-4E21-87BD-693B0C461F93}" name="error bajada (%)" dataDxfId="0">
+      <calculatedColumnFormula>ABS((Tabla312[[#This Row],[Promedio Bajada (ms)]]-Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1629,7 +1926,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1976,12 +2273,2024 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E868A03C-271A-4F8D-9BE9-99D478C798BF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.21875" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="21.77734375" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+    </row>
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2">
+        <v>29.6</v>
+      </c>
+      <c r="C3" s="11">
+        <f>ABS((Tabla3[[#This Row],[Exp Frecuencia (Hz)]]-Tabla3[[#This Row],[Frecuencia (Hz) ]])/Tabla3[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1.3333333333333286E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3.28</v>
+      </c>
+      <c r="F3" s="11">
+        <f>ABS((Tabla3[[#This Row],[Amplitud experimental]]-Tabla3[[#This Row],[Amplitud]])/Tabla3[[#This Row],[Amplitud]])</f>
+        <v>6.0606060606060667E-3</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="I3" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio subida (s)]]-Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2</v>
+      </c>
+      <c r="K3" s="2">
+        <f>Tabla3[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.98</v>
+      </c>
+      <c r="L3" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio Bajada (ms)]]-Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2">
+        <v>29.6</v>
+      </c>
+      <c r="C4" s="11">
+        <f>ABS((Tabla3[[#This Row],[Exp Frecuencia (Hz)]]-Tabla3[[#This Row],[Frecuencia (Hz) ]])/Tabla3[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1.3333333333333286E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="F4" s="11">
+        <f>ABS((Tabla3[[#This Row],[Amplitud experimental]]-Tabla3[[#This Row],[Amplitud]])/Tabla3[[#This Row],[Amplitud]])</f>
+        <v>4.4444444444443499E-3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2.08</v>
+      </c>
+      <c r="I4" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio subida (s)]]-Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2">
+        <f>Tabla3[[#This Row],[Promedio subida (s)]]</f>
+        <v>2.08</v>
+      </c>
+      <c r="L4" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio Bajada (ms)]]-Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>30</v>
+      </c>
+      <c r="B5" s="2">
+        <v>30</v>
+      </c>
+      <c r="C5" s="11">
+        <f>ABS((Tabla3[[#This Row],[Exp Frecuencia (Hz)]]-Tabla3[[#This Row],[Frecuencia (Hz) ]])/Tabla3[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="F5" s="11">
+        <f>ABS((Tabla3[[#This Row],[Amplitud experimental]]-Tabla3[[#This Row],[Amplitud]])/Tabla3[[#This Row],[Amplitud]])</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1.92</v>
+      </c>
+      <c r="I5" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio subida (s)]]-Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
+      <c r="K5" s="2">
+        <f>Tabla3[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.92</v>
+      </c>
+      <c r="L5" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio Bajada (ms)]]-Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2">
+        <v>25.1</v>
+      </c>
+      <c r="C6" s="11">
+        <f>ABS((Tabla3[[#This Row],[Exp Frecuencia (Hz)]]-Tabla3[[#This Row],[Frecuencia (Hz) ]])/Tabla3[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>4.0000000000000565E-3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3.32</v>
+      </c>
+      <c r="F6" s="11">
+        <f>ABS((Tabla3[[#This Row],[Amplitud experimental]]-Tabla3[[#This Row],[Amplitud]])/Tabla3[[#This Row],[Amplitud]])</f>
+        <v>6.0606060606060667E-3</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="I6" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio subida (s)]]-Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2</v>
+      </c>
+      <c r="K6" s="2">
+        <f>Tabla3[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.98</v>
+      </c>
+      <c r="L6" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio Bajada (ms)]]-Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="C7" s="11">
+        <f>ABS((Tabla3[[#This Row],[Exp Frecuencia (Hz)]]-Tabla3[[#This Row],[Frecuencia (Hz) ]])/Tabla3[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>2.4000000000000056E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="F7" s="11">
+        <f>ABS((Tabla3[[#This Row],[Amplitud experimental]]-Tabla3[[#This Row],[Amplitud]])/Tabla3[[#This Row],[Amplitud]])</f>
+        <v>4.4444444444443499E-3</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1.95</v>
+      </c>
+      <c r="I7" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio subida (s)]]-Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>2.5000000000000022E-2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2</v>
+      </c>
+      <c r="K7" s="2">
+        <f>Tabla3[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.95</v>
+      </c>
+      <c r="L7" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio Bajada (ms)]]-Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>2.5000000000000022E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2">
+        <v>25</v>
+      </c>
+      <c r="C8" s="11">
+        <f>ABS((Tabla3[[#This Row],[Exp Frecuencia (Hz)]]-Tabla3[[#This Row],[Frecuencia (Hz) ]])/Tabla3[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="F8" s="11">
+        <f>ABS((Tabla3[[#This Row],[Amplitud experimental]]-Tabla3[[#This Row],[Amplitud]])/Tabla3[[#This Row],[Amplitud]])</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1.94</v>
+      </c>
+      <c r="I8" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio subida (s)]]-Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="J8" s="2">
+        <v>2</v>
+      </c>
+      <c r="K8" s="2">
+        <f>Tabla3[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.94</v>
+      </c>
+      <c r="L8" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio Bajada (ms)]]-Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>3.0000000000000027E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2">
+        <v>19.8</v>
+      </c>
+      <c r="C9" s="11">
+        <f>ABS((Tabla3[[#This Row],[Exp Frecuencia (Hz)]]-Tabla3[[#This Row],[Frecuencia (Hz) ]])/Tabla3[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>9.9999999999999638E-3</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3.33</v>
+      </c>
+      <c r="F9" s="11">
+        <f>ABS((Tabla3[[#This Row],[Amplitud experimental]]-Tabla3[[#This Row],[Amplitud]])/Tabla3[[#This Row],[Amplitud]])</f>
+        <v>9.0909090909091668E-3</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
+      <c r="I9" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio subida (s)]]-Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>2</v>
+      </c>
+      <c r="K9" s="2">
+        <f>Tabla3[[#This Row],[Promedio subida (s)]]</f>
+        <v>2</v>
+      </c>
+      <c r="L9" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio Bajada (ms)]]-Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2">
+        <v>20.5</v>
+      </c>
+      <c r="C10" s="11">
+        <f>ABS((Tabla3[[#This Row],[Exp Frecuencia (Hz)]]-Tabla3[[#This Row],[Frecuencia (Hz) ]])/Tabla3[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F10" s="11">
+        <f>ABS((Tabla3[[#This Row],[Amplitud experimental]]-Tabla3[[#This Row],[Amplitud]])/Tabla3[[#This Row],[Amplitud]])</f>
+        <v>2.2222222222222143E-2</v>
+      </c>
+      <c r="G10" s="2">
+        <v>2</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="I10" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio subida (s)]]-Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="J10" s="2">
+        <v>2</v>
+      </c>
+      <c r="K10" s="2">
+        <f>Tabla3[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.98</v>
+      </c>
+      <c r="L10" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio Bajada (ms)]]-Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="11">
+        <f>ABS((Tabla3[[#This Row],[Exp Frecuencia (Hz)]]-Tabla3[[#This Row],[Frecuencia (Hz) ]])/Tabla3[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.23</v>
+      </c>
+      <c r="F11" s="11">
+        <f>ABS((Tabla3[[#This Row],[Amplitud experimental]]-Tabla3[[#This Row],[Amplitud]])/Tabla3[[#This Row],[Amplitud]])</f>
+        <v>1.6000000000000014E-2</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="I11" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio subida (s)]]-Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="J11" s="2">
+        <v>2</v>
+      </c>
+      <c r="K11" s="2">
+        <f>Tabla3[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.98</v>
+      </c>
+      <c r="L11" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio Bajada (ms)]]-Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="11">
+        <f>ABS((Tabla3[[#This Row],[Exp Frecuencia (Hz)]]-Tabla3[[#This Row],[Frecuencia (Hz) ]])/Tabla3[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="11">
+        <f>ABS((Tabla3[[#This Row],[Amplitud experimental]]-Tabla3[[#This Row],[Amplitud]])/Tabla3[[#This Row],[Amplitud]])</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio subida (s)]]-Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J12" s="2">
+        <v>2</v>
+      </c>
+      <c r="K12" s="2">
+        <f>Tabla3[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio Bajada (ms)]]-Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="11">
+        <f>ABS((Tabla3[[#This Row],[Exp Frecuencia (Hz)]]-Tabla3[[#This Row],[Frecuencia (Hz) ]])/Tabla3[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="11">
+        <f>ABS((Tabla3[[#This Row],[Amplitud experimental]]-Tabla3[[#This Row],[Amplitud]])/Tabla3[[#This Row],[Amplitud]])</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio subida (s)]]-Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J13" s="2">
+        <v>2</v>
+      </c>
+      <c r="K13" s="2">
+        <f>Tabla3[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio Bajada (ms)]]-Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="11">
+        <f>ABS((Tabla3[[#This Row],[Exp Frecuencia (Hz)]]-Tabla3[[#This Row],[Frecuencia (Hz) ]])/Tabla3[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="11">
+        <f>ABS((Tabla3[[#This Row],[Amplitud experimental]]-Tabla3[[#This Row],[Amplitud]])/Tabla3[[#This Row],[Amplitud]])</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio subida (s)]]-Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J14" s="2">
+        <v>2</v>
+      </c>
+      <c r="K14" s="2">
+        <f>Tabla3[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio Bajada (ms)]]-Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="11">
+        <f>ABS((Tabla3[[#This Row],[Exp Frecuencia (Hz)]]-Tabla3[[#This Row],[Frecuencia (Hz) ]])/Tabla3[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="11">
+        <f>ABS((Tabla3[[#This Row],[Amplitud experimental]]-Tabla3[[#This Row],[Amplitud]])/Tabla3[[#This Row],[Amplitud]])</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio subida (s)]]-Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J15" s="2">
+        <v>2</v>
+      </c>
+      <c r="K15" s="2">
+        <f>Tabla3[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio Bajada (ms)]]-Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="11">
+        <f>ABS((Tabla3[[#This Row],[Exp Frecuencia (Hz)]]-Tabla3[[#This Row],[Frecuencia (Hz) ]])/Tabla3[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="11">
+        <f>ABS((Tabla3[[#This Row],[Amplitud experimental]]-Tabla3[[#This Row],[Amplitud]])/Tabla3[[#This Row],[Amplitud]])</f>
+        <v>1</v>
+      </c>
+      <c r="G16" s="2">
+        <v>2</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio subida (s)]]-Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J16" s="2">
+        <v>2</v>
+      </c>
+      <c r="K16" s="2">
+        <f>Tabla3[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio Bajada (ms)]]-Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="11">
+        <f>ABS((Tabla3[[#This Row],[Exp Frecuencia (Hz)]]-Tabla3[[#This Row],[Frecuencia (Hz) ]])/Tabla3[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="11">
+        <f>ABS((Tabla3[[#This Row],[Amplitud experimental]]-Tabla3[[#This Row],[Amplitud]])/Tabla3[[#This Row],[Amplitud]])</f>
+        <v>1</v>
+      </c>
+      <c r="G17" s="2">
+        <v>2</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio subida (s)]]-Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla3[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J17" s="2">
+        <v>2</v>
+      </c>
+      <c r="K17" s="2">
+        <f>Tabla3[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="11">
+        <f>ABS((Tabla3[[#This Row],[Promedio Bajada (ms)]]-Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla3[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+    </row>
+    <row r="22" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>30</v>
+      </c>
+      <c r="B23" s="2">
+        <v>29.4</v>
+      </c>
+      <c r="C23" s="11">
+        <f>ABS((Tabla311[[#This Row],[Exp Frecuencia (Hz)]]-Tabla311[[#This Row],[Frecuencia (Hz) ]])/Tabla311[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>2.0000000000000049E-2</v>
+      </c>
+      <c r="D23" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="E23" s="2">
+        <v>3.36</v>
+      </c>
+      <c r="F23" s="11">
+        <f>ABS((Tabla311[[#This Row],[Amplitud experimental]]-Tabla311[[#This Row],[Amplitud]])/Tabla311[[#This Row],[Amplitud]])</f>
+        <v>1.8181818181818198E-2</v>
+      </c>
+      <c r="G23" s="2">
+        <v>2</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="I23" s="11">
+        <f>ABS((Tabla311[[#This Row],[Promedio subida (s)]]-Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="J23" s="2">
+        <v>2</v>
+      </c>
+      <c r="K23" s="2">
+        <f>Tabla311[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.98</v>
+      </c>
+      <c r="L23" s="10">
+        <f>ABS((Tabla311[[#This Row],[Promedio Bajada (ms)]]-Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>30</v>
+      </c>
+      <c r="B24" s="2">
+        <v>31.4</v>
+      </c>
+      <c r="C24" s="11">
+        <f>ABS((Tabla311[[#This Row],[Exp Frecuencia (Hz)]]-Tabla311[[#This Row],[Frecuencia (Hz) ]])/Tabla311[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>4.666666666666662E-2</v>
+      </c>
+      <c r="D24" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2.23</v>
+      </c>
+      <c r="F24" s="11">
+        <f>ABS((Tabla311[[#This Row],[Amplitud experimental]]-Tabla311[[#This Row],[Amplitud]])/Tabla311[[#This Row],[Amplitud]])</f>
+        <v>8.8888888888888976E-3</v>
+      </c>
+      <c r="G24" s="2">
+        <v>2</v>
+      </c>
+      <c r="H24" s="2">
+        <v>2.08</v>
+      </c>
+      <c r="I24" s="11">
+        <f>ABS((Tabla311[[#This Row],[Promedio subida (s)]]-Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="J24" s="2">
+        <v>2</v>
+      </c>
+      <c r="K24" s="2">
+        <f>Tabla311[[#This Row],[Promedio subida (s)]]</f>
+        <v>2.08</v>
+      </c>
+      <c r="L24" s="10">
+        <f>ABS((Tabla311[[#This Row],[Promedio Bajada (ms)]]-Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>30</v>
+      </c>
+      <c r="B25" s="2">
+        <v>28.9</v>
+      </c>
+      <c r="C25" s="11">
+        <f>ABS((Tabla311[[#This Row],[Exp Frecuencia (Hz)]]-Tabla311[[#This Row],[Frecuencia (Hz) ]])/Tabla311[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>3.6666666666666715E-2</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1.24</v>
+      </c>
+      <c r="F25" s="11">
+        <f>ABS((Tabla311[[#This Row],[Amplitud experimental]]-Tabla311[[#This Row],[Amplitud]])/Tabla311[[#This Row],[Amplitud]])</f>
+        <v>8.0000000000000071E-3</v>
+      </c>
+      <c r="G25" s="2">
+        <v>2</v>
+      </c>
+      <c r="H25" s="2">
+        <v>1.92</v>
+      </c>
+      <c r="I25" s="11">
+        <f>ABS((Tabla311[[#This Row],[Promedio subida (s)]]-Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="J25" s="2">
+        <v>2</v>
+      </c>
+      <c r="K25" s="2">
+        <f>Tabla311[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.92</v>
+      </c>
+      <c r="L25" s="10">
+        <f>ABS((Tabla311[[#This Row],[Promedio Bajada (ms)]]-Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>25.1</v>
+      </c>
+      <c r="C26" s="11">
+        <f>ABS((Tabla311[[#This Row],[Exp Frecuencia (Hz)]]-Tabla311[[#This Row],[Frecuencia (Hz) ]])/Tabla311[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>4.0000000000000565E-3</v>
+      </c>
+      <c r="D26" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="E26" s="2">
+        <v>3.32</v>
+      </c>
+      <c r="F26" s="11">
+        <f>ABS((Tabla311[[#This Row],[Amplitud experimental]]-Tabla311[[#This Row],[Amplitud]])/Tabla311[[#This Row],[Amplitud]])</f>
+        <v>6.0606060606060667E-3</v>
+      </c>
+      <c r="G26" s="2">
+        <v>2</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="I26" s="11">
+        <f>ABS((Tabla311[[#This Row],[Promedio subida (s)]]-Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="J26" s="2">
+        <v>2</v>
+      </c>
+      <c r="K26" s="2">
+        <f>Tabla311[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.98</v>
+      </c>
+      <c r="L26" s="10">
+        <f>ABS((Tabla311[[#This Row],[Promedio Bajada (ms)]]-Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2">
+        <v>25.1</v>
+      </c>
+      <c r="C27" s="11">
+        <f>ABS((Tabla311[[#This Row],[Exp Frecuencia (Hz)]]-Tabla311[[#This Row],[Frecuencia (Hz) ]])/Tabla311[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>4.0000000000000565E-3</v>
+      </c>
+      <c r="D27" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="F27" s="11">
+        <f>ABS((Tabla311[[#This Row],[Amplitud experimental]]-Tabla311[[#This Row],[Amplitud]])/Tabla311[[#This Row],[Amplitud]])</f>
+        <v>4.4444444444443499E-3</v>
+      </c>
+      <c r="G27" s="2">
+        <v>2</v>
+      </c>
+      <c r="H27" s="2">
+        <v>1.95</v>
+      </c>
+      <c r="I27" s="11">
+        <f>ABS((Tabla311[[#This Row],[Promedio subida (s)]]-Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>2.5000000000000022E-2</v>
+      </c>
+      <c r="J27" s="2">
+        <v>2</v>
+      </c>
+      <c r="K27" s="2">
+        <f>Tabla311[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.95</v>
+      </c>
+      <c r="L27" s="10">
+        <f>ABS((Tabla311[[#This Row],[Promedio Bajada (ms)]]-Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>2.5000000000000022E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>25</v>
+      </c>
+      <c r="B28" s="2">
+        <v>25</v>
+      </c>
+      <c r="C28" s="11">
+        <f>ABS((Tabla311[[#This Row],[Exp Frecuencia (Hz)]]-Tabla311[[#This Row],[Frecuencia (Hz) ]])/Tabla311[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1.23</v>
+      </c>
+      <c r="F28" s="11">
+        <f>ABS((Tabla311[[#This Row],[Amplitud experimental]]-Tabla311[[#This Row],[Amplitud]])/Tabla311[[#This Row],[Amplitud]])</f>
+        <v>1.6000000000000014E-2</v>
+      </c>
+      <c r="G28" s="2">
+        <v>2</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1.94</v>
+      </c>
+      <c r="I28" s="11">
+        <f>ABS((Tabla311[[#This Row],[Promedio subida (s)]]-Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="J28" s="2">
+        <v>2</v>
+      </c>
+      <c r="K28" s="2">
+        <f>Tabla311[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.94</v>
+      </c>
+      <c r="L28" s="10">
+        <f>ABS((Tabla311[[#This Row],[Promedio Bajada (ms)]]-Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>3.0000000000000027E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>20</v>
+      </c>
+      <c r="B29" s="2">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="C29" s="11">
+        <f>ABS((Tabla311[[#This Row],[Exp Frecuencia (Hz)]]-Tabla311[[#This Row],[Frecuencia (Hz) ]])/Tabla311[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>5.0000000000000712E-3</v>
+      </c>
+      <c r="D29" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="E29" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="F29" s="11">
+        <f>ABS((Tabla311[[#This Row],[Amplitud experimental]]-Tabla311[[#This Row],[Amplitud]])/Tabla311[[#This Row],[Amplitud]])</f>
+        <v>3.0303030303030196E-2</v>
+      </c>
+      <c r="G29" s="2">
+        <v>2</v>
+      </c>
+      <c r="H29" s="2">
+        <v>2</v>
+      </c>
+      <c r="I29" s="11">
+        <f>ABS((Tabla311[[#This Row],[Promedio subida (s)]]-Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="2">
+        <v>2</v>
+      </c>
+      <c r="K29" s="2">
+        <f>Tabla311[[#This Row],[Promedio subida (s)]]</f>
+        <v>2</v>
+      </c>
+      <c r="L29" s="10">
+        <f>ABS((Tabla311[[#This Row],[Promedio Bajada (ms)]]-Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>20</v>
+      </c>
+      <c r="B30" s="2">
+        <v>20.3</v>
+      </c>
+      <c r="C30" s="11">
+        <f>ABS((Tabla311[[#This Row],[Exp Frecuencia (Hz)]]-Tabla311[[#This Row],[Frecuencia (Hz) ]])/Tabla311[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1.5000000000000036E-2</v>
+      </c>
+      <c r="D30" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="E30" s="2">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="F30" s="11">
+        <f>ABS((Tabla311[[#This Row],[Amplitud experimental]]-Tabla311[[#This Row],[Amplitud]])/Tabla311[[#This Row],[Amplitud]])</f>
+        <v>1.3333333333333246E-2</v>
+      </c>
+      <c r="G30" s="2">
+        <v>2</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="I30" s="11">
+        <f>ABS((Tabla311[[#This Row],[Promedio subida (s)]]-Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="J30" s="2">
+        <v>2</v>
+      </c>
+      <c r="K30" s="2">
+        <f>Tabla311[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.98</v>
+      </c>
+      <c r="L30" s="10">
+        <f>ABS((Tabla311[[#This Row],[Promedio Bajada (ms)]]-Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>20</v>
+      </c>
+      <c r="B31" s="2">
+        <v>20.2</v>
+      </c>
+      <c r="C31" s="11">
+        <f>ABS((Tabla311[[#This Row],[Exp Frecuencia (Hz)]]-Tabla311[[#This Row],[Frecuencia (Hz) ]])/Tabla311[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>9.9999999999999638E-3</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E31" s="2">
+        <v>1.24</v>
+      </c>
+      <c r="F31" s="11">
+        <f>ABS((Tabla311[[#This Row],[Amplitud experimental]]-Tabla311[[#This Row],[Amplitud]])/Tabla311[[#This Row],[Amplitud]])</f>
+        <v>8.0000000000000071E-3</v>
+      </c>
+      <c r="G31" s="2">
+        <v>2</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1.99</v>
+      </c>
+      <c r="I31" s="11">
+        <f>ABS((Tabla311[[#This Row],[Promedio subida (s)]]-Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>5.0000000000000044E-3</v>
+      </c>
+      <c r="J31" s="2">
+        <v>2</v>
+      </c>
+      <c r="K31" s="2">
+        <f>Tabla311[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.99</v>
+      </c>
+      <c r="L31" s="10">
+        <f>ABS((Tabla311[[#This Row],[Promedio Bajada (ms)]]-Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>5.0000000000000044E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>15</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="11">
+        <f>ABS((Tabla311[[#This Row],[Exp Frecuencia (Hz)]]-Tabla311[[#This Row],[Frecuencia (Hz) ]])/Tabla311[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D32" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="11">
+        <f>ABS((Tabla311[[#This Row],[Amplitud experimental]]-Tabla311[[#This Row],[Amplitud]])/Tabla311[[#This Row],[Amplitud]])</f>
+        <v>1</v>
+      </c>
+      <c r="G32" s="2">
+        <v>2</v>
+      </c>
+      <c r="H32" s="2"/>
+      <c r="I32" s="11">
+        <f>ABS((Tabla311[[#This Row],[Promedio subida (s)]]-Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J32" s="2">
+        <v>2</v>
+      </c>
+      <c r="K32" s="2">
+        <f>Tabla311[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L32" s="10">
+        <f>ABS((Tabla311[[#This Row],[Promedio Bajada (ms)]]-Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>15</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="11">
+        <f>ABS((Tabla311[[#This Row],[Exp Frecuencia (Hz)]]-Tabla311[[#This Row],[Frecuencia (Hz) ]])/Tabla311[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D33" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="11">
+        <f>ABS((Tabla311[[#This Row],[Amplitud experimental]]-Tabla311[[#This Row],[Amplitud]])/Tabla311[[#This Row],[Amplitud]])</f>
+        <v>1</v>
+      </c>
+      <c r="G33" s="2">
+        <v>2</v>
+      </c>
+      <c r="H33" s="2"/>
+      <c r="I33" s="11">
+        <f>ABS((Tabla311[[#This Row],[Promedio subida (s)]]-Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J33" s="2">
+        <v>2</v>
+      </c>
+      <c r="K33" s="2">
+        <f>Tabla311[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L33" s="10">
+        <f>ABS((Tabla311[[#This Row],[Promedio Bajada (ms)]]-Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>15</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="11">
+        <f>ABS((Tabla311[[#This Row],[Exp Frecuencia (Hz)]]-Tabla311[[#This Row],[Frecuencia (Hz) ]])/Tabla311[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="11">
+        <f>ABS((Tabla311[[#This Row],[Amplitud experimental]]-Tabla311[[#This Row],[Amplitud]])/Tabla311[[#This Row],[Amplitud]])</f>
+        <v>1</v>
+      </c>
+      <c r="G34" s="2">
+        <v>2</v>
+      </c>
+      <c r="H34" s="2"/>
+      <c r="I34" s="11">
+        <f>ABS((Tabla311[[#This Row],[Promedio subida (s)]]-Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J34" s="2">
+        <v>2</v>
+      </c>
+      <c r="K34" s="2">
+        <f>Tabla311[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L34" s="10">
+        <f>ABS((Tabla311[[#This Row],[Promedio Bajada (ms)]]-Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>10</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="11">
+        <f>ABS((Tabla311[[#This Row],[Exp Frecuencia (Hz)]]-Tabla311[[#This Row],[Frecuencia (Hz) ]])/Tabla311[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D35" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="11">
+        <f>ABS((Tabla311[[#This Row],[Amplitud experimental]]-Tabla311[[#This Row],[Amplitud]])/Tabla311[[#This Row],[Amplitud]])</f>
+        <v>1</v>
+      </c>
+      <c r="G35" s="2">
+        <v>2</v>
+      </c>
+      <c r="H35" s="2"/>
+      <c r="I35" s="11">
+        <f>ABS((Tabla311[[#This Row],[Promedio subida (s)]]-Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J35" s="2">
+        <v>2</v>
+      </c>
+      <c r="K35" s="2">
+        <f>Tabla311[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="10">
+        <f>ABS((Tabla311[[#This Row],[Promedio Bajada (ms)]]-Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>10</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="11">
+        <f>ABS((Tabla311[[#This Row],[Exp Frecuencia (Hz)]]-Tabla311[[#This Row],[Frecuencia (Hz) ]])/Tabla311[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D36" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="11">
+        <f>ABS((Tabla311[[#This Row],[Amplitud experimental]]-Tabla311[[#This Row],[Amplitud]])/Tabla311[[#This Row],[Amplitud]])</f>
+        <v>1</v>
+      </c>
+      <c r="G36" s="2">
+        <v>2</v>
+      </c>
+      <c r="H36" s="2"/>
+      <c r="I36" s="11">
+        <f>ABS((Tabla311[[#This Row],[Promedio subida (s)]]-Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J36" s="2">
+        <v>2</v>
+      </c>
+      <c r="K36" s="2">
+        <f>Tabla311[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L36" s="10">
+        <f>ABS((Tabla311[[#This Row],[Promedio Bajada (ms)]]-Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>10</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="11">
+        <f>ABS((Tabla311[[#This Row],[Exp Frecuencia (Hz)]]-Tabla311[[#This Row],[Frecuencia (Hz) ]])/Tabla311[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="11">
+        <f>ABS((Tabla311[[#This Row],[Amplitud experimental]]-Tabla311[[#This Row],[Amplitud]])/Tabla311[[#This Row],[Amplitud]])</f>
+        <v>1</v>
+      </c>
+      <c r="G37" s="2">
+        <v>2</v>
+      </c>
+      <c r="H37" s="2"/>
+      <c r="I37" s="11">
+        <f>ABS((Tabla311[[#This Row],[Promedio subida (s)]]-Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla311[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J37" s="2">
+        <v>2</v>
+      </c>
+      <c r="K37" s="2">
+        <f>Tabla311[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L37" s="10">
+        <f>ABS((Tabla311[[#This Row],[Promedio Bajada (ms)]]-Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla311[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+    </row>
+    <row r="41" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>30</v>
+      </c>
+      <c r="B42" s="2">
+        <v>29.6</v>
+      </c>
+      <c r="C42" s="11">
+        <f>ABS((Tabla312[[#This Row],[Exp Frecuencia (Hz)]]-Tabla312[[#This Row],[Frecuencia (Hz) ]])/Tabla312[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1.3333333333333286E-2</v>
+      </c>
+      <c r="D42" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="E42" s="2">
+        <v>3.28</v>
+      </c>
+      <c r="F42" s="11">
+        <f>ABS((Tabla312[[#This Row],[Amplitud experimental]]-Tabla312[[#This Row],[Amplitud]])/Tabla312[[#This Row],[Amplitud]])</f>
+        <v>6.0606060606060667E-3</v>
+      </c>
+      <c r="G42" s="2">
+        <v>2</v>
+      </c>
+      <c r="H42" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="I42" s="11">
+        <f>ABS((Tabla312[[#This Row],[Promedio subida (s)]]-Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="J42" s="2">
+        <v>2</v>
+      </c>
+      <c r="K42" s="2">
+        <f>Tabla312[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.98</v>
+      </c>
+      <c r="L42" s="10">
+        <f>ABS((Tabla312[[#This Row],[Promedio Bajada (ms)]]-Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>30</v>
+      </c>
+      <c r="B43" s="2">
+        <v>29.4</v>
+      </c>
+      <c r="C43" s="11">
+        <f>ABS((Tabla312[[#This Row],[Exp Frecuencia (Hz)]]-Tabla312[[#This Row],[Frecuencia (Hz) ]])/Tabla312[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>2.0000000000000049E-2</v>
+      </c>
+      <c r="D43" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="E43" s="2">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="F43" s="11">
+        <f>ABS((Tabla312[[#This Row],[Amplitud experimental]]-Tabla312[[#This Row],[Amplitud]])/Tabla312[[#This Row],[Amplitud]])</f>
+        <v>4.4444444444443499E-3</v>
+      </c>
+      <c r="G43" s="2">
+        <v>2</v>
+      </c>
+      <c r="H43" s="2">
+        <v>2.08</v>
+      </c>
+      <c r="I43" s="11">
+        <f>ABS((Tabla312[[#This Row],[Promedio subida (s)]]-Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="J43" s="2">
+        <v>2</v>
+      </c>
+      <c r="K43" s="2">
+        <f>Tabla312[[#This Row],[Promedio subida (s)]]</f>
+        <v>2.08</v>
+      </c>
+      <c r="L43" s="10">
+        <f>ABS((Tabla312[[#This Row],[Promedio Bajada (ms)]]-Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>30</v>
+      </c>
+      <c r="B44" s="2">
+        <v>28.8</v>
+      </c>
+      <c r="C44" s="11">
+        <f>ABS((Tabla312[[#This Row],[Exp Frecuencia (Hz)]]-Tabla312[[#This Row],[Frecuencia (Hz) ]])/Tabla312[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>3.9999999999999973E-2</v>
+      </c>
+      <c r="D44" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="F44" s="11">
+        <f>ABS((Tabla312[[#This Row],[Amplitud experimental]]-Tabla312[[#This Row],[Amplitud]])/Tabla312[[#This Row],[Amplitud]])</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="G44" s="2">
+        <v>2</v>
+      </c>
+      <c r="H44" s="2">
+        <v>1.92</v>
+      </c>
+      <c r="I44" s="11">
+        <f>ABS((Tabla312[[#This Row],[Promedio subida (s)]]-Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="J44" s="2">
+        <v>2</v>
+      </c>
+      <c r="K44" s="2">
+        <f>Tabla312[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.92</v>
+      </c>
+      <c r="L44" s="10">
+        <f>ABS((Tabla312[[#This Row],[Promedio Bajada (ms)]]-Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>25</v>
+      </c>
+      <c r="B45" s="2">
+        <v>25.2</v>
+      </c>
+      <c r="C45" s="11">
+        <f>ABS((Tabla312[[#This Row],[Exp Frecuencia (Hz)]]-Tabla312[[#This Row],[Frecuencia (Hz) ]])/Tabla312[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>7.9999999999999724E-3</v>
+      </c>
+      <c r="D45" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="E45" s="2">
+        <v>3.33</v>
+      </c>
+      <c r="F45" s="11">
+        <f>ABS((Tabla312[[#This Row],[Amplitud experimental]]-Tabla312[[#This Row],[Amplitud]])/Tabla312[[#This Row],[Amplitud]])</f>
+        <v>9.0909090909091668E-3</v>
+      </c>
+      <c r="G45" s="2">
+        <v>2</v>
+      </c>
+      <c r="H45" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="I45" s="11">
+        <f>ABS((Tabla312[[#This Row],[Promedio subida (s)]]-Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="J45" s="2">
+        <v>2</v>
+      </c>
+      <c r="K45" s="2">
+        <f>Tabla312[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.98</v>
+      </c>
+      <c r="L45" s="10">
+        <f>ABS((Tabla312[[#This Row],[Promedio Bajada (ms)]]-Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>25</v>
+      </c>
+      <c r="B46" s="2">
+        <v>24.8</v>
+      </c>
+      <c r="C46" s="11">
+        <f>ABS((Tabla312[[#This Row],[Exp Frecuencia (Hz)]]-Tabla312[[#This Row],[Frecuencia (Hz) ]])/Tabla312[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>7.9999999999999724E-3</v>
+      </c>
+      <c r="D46" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="E46" s="2">
+        <v>2.23</v>
+      </c>
+      <c r="F46" s="11">
+        <f>ABS((Tabla312[[#This Row],[Amplitud experimental]]-Tabla312[[#This Row],[Amplitud]])/Tabla312[[#This Row],[Amplitud]])</f>
+        <v>8.8888888888888976E-3</v>
+      </c>
+      <c r="G46" s="2">
+        <v>2</v>
+      </c>
+      <c r="H46" s="2">
+        <v>1.95</v>
+      </c>
+      <c r="I46" s="11">
+        <f>ABS((Tabla312[[#This Row],[Promedio subida (s)]]-Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>2.5000000000000022E-2</v>
+      </c>
+      <c r="J46" s="2">
+        <v>2</v>
+      </c>
+      <c r="K46" s="2">
+        <f>Tabla312[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.95</v>
+      </c>
+      <c r="L46" s="10">
+        <f>ABS((Tabla312[[#This Row],[Promedio Bajada (ms)]]-Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>2.5000000000000022E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>25</v>
+      </c>
+      <c r="B47" s="2">
+        <v>25</v>
+      </c>
+      <c r="C47" s="11">
+        <f>ABS((Tabla312[[#This Row],[Exp Frecuencia (Hz)]]-Tabla312[[#This Row],[Frecuencia (Hz) ]])/Tabla312[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>0</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E47" s="2">
+        <v>1.23</v>
+      </c>
+      <c r="F47" s="11">
+        <f>ABS((Tabla312[[#This Row],[Amplitud experimental]]-Tabla312[[#This Row],[Amplitud]])/Tabla312[[#This Row],[Amplitud]])</f>
+        <v>1.6000000000000014E-2</v>
+      </c>
+      <c r="G47" s="2">
+        <v>2</v>
+      </c>
+      <c r="H47" s="2">
+        <v>1.94</v>
+      </c>
+      <c r="I47" s="11">
+        <f>ABS((Tabla312[[#This Row],[Promedio subida (s)]]-Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="J47" s="2">
+        <v>2</v>
+      </c>
+      <c r="K47" s="2">
+        <f>Tabla312[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.94</v>
+      </c>
+      <c r="L47" s="10">
+        <f>ABS((Tabla312[[#This Row],[Promedio Bajada (ms)]]-Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>3.0000000000000027E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>20</v>
+      </c>
+      <c r="B48" s="2">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="C48" s="11">
+        <f>ABS((Tabla312[[#This Row],[Exp Frecuencia (Hz)]]-Tabla312[[#This Row],[Frecuencia (Hz) ]])/Tabla312[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>5.0000000000000712E-3</v>
+      </c>
+      <c r="D48" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="E48" s="2">
+        <v>3.33</v>
+      </c>
+      <c r="F48" s="11">
+        <f>ABS((Tabla312[[#This Row],[Amplitud experimental]]-Tabla312[[#This Row],[Amplitud]])/Tabla312[[#This Row],[Amplitud]])</f>
+        <v>9.0909090909091668E-3</v>
+      </c>
+      <c r="G48" s="2">
+        <v>2</v>
+      </c>
+      <c r="H48" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="I48" s="11">
+        <f>ABS((Tabla312[[#This Row],[Promedio subida (s)]]-Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="J48" s="2">
+        <v>2</v>
+      </c>
+      <c r="K48" s="2">
+        <f>Tabla312[[#This Row],[Promedio subida (s)]]</f>
+        <v>1.98</v>
+      </c>
+      <c r="L48" s="10">
+        <f>ABS((Tabla312[[#This Row],[Promedio Bajada (ms)]]-Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1.0000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>20</v>
+      </c>
+      <c r="B49" s="2">
+        <v>20.2</v>
+      </c>
+      <c r="C49" s="11">
+        <f>ABS((Tabla312[[#This Row],[Exp Frecuencia (Hz)]]-Tabla312[[#This Row],[Frecuencia (Hz) ]])/Tabla312[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>9.9999999999999638E-3</v>
+      </c>
+      <c r="D49" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="E49" s="2">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="F49" s="11">
+        <f>ABS((Tabla312[[#This Row],[Amplitud experimental]]-Tabla312[[#This Row],[Amplitud]])/Tabla312[[#This Row],[Amplitud]])</f>
+        <v>4.4444444444443499E-3</v>
+      </c>
+      <c r="G49" s="2">
+        <v>2</v>
+      </c>
+      <c r="H49" s="2">
+        <v>2</v>
+      </c>
+      <c r="I49" s="11">
+        <f>ABS((Tabla312[[#This Row],[Promedio subida (s)]]-Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>0</v>
+      </c>
+      <c r="J49" s="2">
+        <v>2</v>
+      </c>
+      <c r="K49" s="2">
+        <f>Tabla312[[#This Row],[Promedio subida (s)]]</f>
+        <v>2</v>
+      </c>
+      <c r="L49" s="10">
+        <f>ABS((Tabla312[[#This Row],[Promedio Bajada (ms)]]-Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>20</v>
+      </c>
+      <c r="B50" s="2">
+        <v>20.2</v>
+      </c>
+      <c r="C50" s="11">
+        <f>ABS((Tabla312[[#This Row],[Exp Frecuencia (Hz)]]-Tabla312[[#This Row],[Frecuencia (Hz) ]])/Tabla312[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>9.9999999999999638E-3</v>
+      </c>
+      <c r="D50" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E50" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="F50" s="11">
+        <f>ABS((Tabla312[[#This Row],[Amplitud experimental]]-Tabla312[[#This Row],[Amplitud]])/Tabla312[[#This Row],[Amplitud]])</f>
+        <v>0</v>
+      </c>
+      <c r="G50" s="2">
+        <v>2</v>
+      </c>
+      <c r="H50" s="2"/>
+      <c r="I50" s="11">
+        <f>ABS((Tabla312[[#This Row],[Promedio subida (s)]]-Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J50" s="2">
+        <v>2</v>
+      </c>
+      <c r="K50" s="2">
+        <f>Tabla312[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L50" s="10">
+        <f>ABS((Tabla312[[#This Row],[Promedio Bajada (ms)]]-Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>15</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="11">
+        <f>ABS((Tabla312[[#This Row],[Exp Frecuencia (Hz)]]-Tabla312[[#This Row],[Frecuencia (Hz) ]])/Tabla312[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D51" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="11">
+        <f>ABS((Tabla312[[#This Row],[Amplitud experimental]]-Tabla312[[#This Row],[Amplitud]])/Tabla312[[#This Row],[Amplitud]])</f>
+        <v>1</v>
+      </c>
+      <c r="G51" s="2">
+        <v>2</v>
+      </c>
+      <c r="H51" s="2"/>
+      <c r="I51" s="11">
+        <f>ABS((Tabla312[[#This Row],[Promedio subida (s)]]-Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J51" s="2">
+        <v>2</v>
+      </c>
+      <c r="K51" s="2">
+        <f>Tabla312[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L51" s="10">
+        <f>ABS((Tabla312[[#This Row],[Promedio Bajada (ms)]]-Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>15</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" s="11">
+        <f>ABS((Tabla312[[#This Row],[Exp Frecuencia (Hz)]]-Tabla312[[#This Row],[Frecuencia (Hz) ]])/Tabla312[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D52" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" s="11">
+        <f>ABS((Tabla312[[#This Row],[Amplitud experimental]]-Tabla312[[#This Row],[Amplitud]])/Tabla312[[#This Row],[Amplitud]])</f>
+        <v>1</v>
+      </c>
+      <c r="G52" s="2">
+        <v>2</v>
+      </c>
+      <c r="H52" s="2"/>
+      <c r="I52" s="11">
+        <f>ABS((Tabla312[[#This Row],[Promedio subida (s)]]-Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J52" s="2">
+        <v>2</v>
+      </c>
+      <c r="K52" s="2">
+        <f>Tabla312[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L52" s="10">
+        <f>ABS((Tabla312[[#This Row],[Promedio Bajada (ms)]]-Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>15</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="11">
+        <f>ABS((Tabla312[[#This Row],[Exp Frecuencia (Hz)]]-Tabla312[[#This Row],[Frecuencia (Hz) ]])/Tabla312[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D53" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="11">
+        <f>ABS((Tabla312[[#This Row],[Amplitud experimental]]-Tabla312[[#This Row],[Amplitud]])/Tabla312[[#This Row],[Amplitud]])</f>
+        <v>1</v>
+      </c>
+      <c r="G53" s="2">
+        <v>2</v>
+      </c>
+      <c r="H53" s="2"/>
+      <c r="I53" s="11">
+        <f>ABS((Tabla312[[#This Row],[Promedio subida (s)]]-Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J53" s="2">
+        <v>2</v>
+      </c>
+      <c r="K53" s="2">
+        <f>Tabla312[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L53" s="10">
+        <f>ABS((Tabla312[[#This Row],[Promedio Bajada (ms)]]-Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>10</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" s="11">
+        <f>ABS((Tabla312[[#This Row],[Exp Frecuencia (Hz)]]-Tabla312[[#This Row],[Frecuencia (Hz) ]])/Tabla312[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D54" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="11">
+        <f>ABS((Tabla312[[#This Row],[Amplitud experimental]]-Tabla312[[#This Row],[Amplitud]])/Tabla312[[#This Row],[Amplitud]])</f>
+        <v>1</v>
+      </c>
+      <c r="G54" s="2">
+        <v>2</v>
+      </c>
+      <c r="H54" s="2"/>
+      <c r="I54" s="11">
+        <f>ABS((Tabla312[[#This Row],[Promedio subida (s)]]-Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J54" s="2">
+        <v>2</v>
+      </c>
+      <c r="K54" s="2">
+        <f>Tabla312[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L54" s="10">
+        <f>ABS((Tabla312[[#This Row],[Promedio Bajada (ms)]]-Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>10</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="11">
+        <f>ABS((Tabla312[[#This Row],[Exp Frecuencia (Hz)]]-Tabla312[[#This Row],[Frecuencia (Hz) ]])/Tabla312[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D55" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="E55" s="2"/>
+      <c r="F55" s="11">
+        <f>ABS((Tabla312[[#This Row],[Amplitud experimental]]-Tabla312[[#This Row],[Amplitud]])/Tabla312[[#This Row],[Amplitud]])</f>
+        <v>1</v>
+      </c>
+      <c r="G55" s="2">
+        <v>2</v>
+      </c>
+      <c r="H55" s="2"/>
+      <c r="I55" s="11">
+        <f>ABS((Tabla312[[#This Row],[Promedio subida (s)]]-Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J55" s="2">
+        <v>2</v>
+      </c>
+      <c r="K55" s="2">
+        <f>Tabla312[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L55" s="10">
+        <f>ABS((Tabla312[[#This Row],[Promedio Bajada (ms)]]-Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>10</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="11">
+        <f>ABS((Tabla312[[#This Row],[Exp Frecuencia (Hz)]]-Tabla312[[#This Row],[Frecuencia (Hz) ]])/Tabla312[[#This Row],[Frecuencia (Hz) ]])</f>
+        <v>1</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="11">
+        <f>ABS((Tabla312[[#This Row],[Amplitud experimental]]-Tabla312[[#This Row],[Amplitud]])/Tabla312[[#This Row],[Amplitud]])</f>
+        <v>1</v>
+      </c>
+      <c r="G56" s="2">
+        <v>2</v>
+      </c>
+      <c r="H56" s="2"/>
+      <c r="I56" s="11">
+        <f>ABS((Tabla312[[#This Row],[Promedio subida (s)]]-Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])/Tabla312[[#This Row],[Tiempo Rampa Subida Teorico (s)]])</f>
+        <v>1</v>
+      </c>
+      <c r="J56" s="2">
+        <v>2</v>
+      </c>
+      <c r="K56" s="2">
+        <f>Tabla312[[#This Row],[Promedio subida (s)]]</f>
+        <v>0</v>
+      </c>
+      <c r="L56" s="10">
+        <f>ABS((Tabla312[[#This Row],[Promedio Bajada (ms)]]-Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])/Tabla312[[#This Row],[Tiempo Rampa Bajada (s)]])</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A40:L40"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>